<commit_message>
small fixes for run*.py to conform to previous rivus.py updates
</commit_message>
<xml_diff>
--- a/data/mnl/data.xlsx
+++ b/data/mnl/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" activeTab="2"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="73">
   <si>
     <t>Commodity</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>weight</t>
-  </si>
-  <si>
-    <t>scale</t>
   </si>
   <si>
     <t>peak</t>
@@ -319,10 +316,13 @@
     <t>t high</t>
   </si>
   <si>
-    <t>hours</t>
-  </si>
-  <si>
     <t>cost-fix</t>
+  </si>
+  <si>
+    <t>allowed-max</t>
+  </si>
+  <si>
+    <t>inf</t>
   </si>
 </sst>
 </file>
@@ -330,7 +330,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -509,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -534,8 +534,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -554,6 +554,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -915,7 +918,7 @@
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="14"/>
       <c r="C3" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
@@ -928,7 +931,7 @@
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="14"/>
       <c r="C4" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
@@ -963,7 +966,7 @@
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="19"/>
       <c r="C7" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -976,11 +979,11 @@
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="19"/>
       <c r="C8" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
@@ -991,11 +994,11 @@
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="19"/>
       <c r="C9" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
@@ -1006,11 +1009,11 @@
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="19"/>
       <c r="C10" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -1021,11 +1024,11 @@
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="19"/>
       <c r="C11" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
@@ -1036,11 +1039,11 @@
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="19"/>
       <c r="C12" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -1062,7 +1065,7 @@
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="19"/>
       <c r="C14" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -1075,11 +1078,11 @@
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="19"/>
       <c r="C15" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
@@ -1090,11 +1093,11 @@
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="19"/>
       <c r="C16" s="26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
@@ -1105,11 +1108,11 @@
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="19"/>
       <c r="C17" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
@@ -1246,13 +1249,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,10 +1264,12 @@
     <col min="2" max="5" width="11.42578125" style="3"/>
     <col min="6" max="6" width="11.42578125" style="6"/>
     <col min="7" max="8" width="11.42578125" style="8"/>
-    <col min="9" max="16384" width="11.42578125" style="3"/>
+    <col min="9" max="9" width="11.42578125" style="3"/>
+    <col min="10" max="10" width="12.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1278,22 +1283,25 @@
         <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1321,8 +1329,12 @@
       <c r="I2" s="3">
         <v>750000</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="29" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1350,8 +1362,12 @@
       <c r="I3" s="3">
         <v>500000</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="29" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1379,8 +1395,12 @@
       <c r="I4" s="3">
         <v>160000</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="29" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1408,8 +1428,12 @@
       <c r="I5" s="3">
         <v>90000</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="29" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1444,10 +1468,13 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
@@ -1471,6 +1498,10 @@
         <v>0</v>
       </c>
       <c r="I7" s="29" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J7" s="29" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
@@ -1490,7 +1521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1517,7 +1548,7 @@
         <v>16</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>9</v>
@@ -1529,12 +1560,12 @@
         <v>18</v>
       </c>
       <c r="I1" s="33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="32">
         <v>10000</v>
@@ -1555,12 +1586,12 @@
         <v>600000</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="32">
         <v>15000</v>
@@ -1581,12 +1612,12 @@
         <v>600000</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="32">
         <v>0</v>
@@ -1607,12 +1638,12 @@
         <v>1000</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="32">
         <v>5000</v>
@@ -1633,12 +1664,12 @@
         <v>150000</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="32">
         <v>8000</v>
@@ -1659,12 +1690,12 @@
         <v>400000</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="32">
         <v>5000</v>
@@ -1685,12 +1716,12 @@
         <v>999990</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="32">
         <v>0</v>
@@ -1711,12 +1742,12 @@
         <v>1000</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="32">
         <v>9000</v>
@@ -1737,7 +1768,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1789,7 +1820,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -1803,7 +1834,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -1817,7 +1848,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -1831,7 +1862,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
@@ -1845,7 +1876,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
@@ -1859,7 +1890,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
@@ -1873,7 +1904,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
@@ -1887,7 +1918,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
@@ -1901,7 +1932,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>2</v>
@@ -1915,7 +1946,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
@@ -1929,7 +1960,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>2</v>
@@ -1943,7 +1974,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>4</v>
@@ -1957,7 +1988,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>1</v>
@@ -1971,7 +2002,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>2</v>
@@ -1985,7 +2016,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
@@ -1999,7 +2030,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>1</v>
@@ -2013,7 +2044,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>4</v>
@@ -2027,7 +2058,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
@@ -2041,7 +2072,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>1</v>
@@ -2055,7 +2086,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>4</v>
@@ -2069,7 +2100,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>7</v>
@@ -2083,10 +2114,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>12</v>
@@ -2097,7 +2128,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>4</v>
@@ -2111,7 +2142,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>2</v>
@@ -2125,7 +2156,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>7</v>
@@ -2189,9 +2220,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2202,11 +2233,12 @@
   <cols>
     <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="3"/>
-    <col min="3" max="3" width="11.42578125" style="6"/>
-    <col min="4" max="16384" width="11.42578125" style="3"/>
+    <col min="3" max="3" width="7.85546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2214,75 +2246,71 @@
         <v>20</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="32">
-        <f>D2</f>
         <v>60</v>
       </c>
       <c r="C2" s="6">
         <v>1</v>
       </c>
-      <c r="D2" s="32">
-        <v>60</v>
-      </c>
-      <c r="G2" s="32"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="32"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="32">
-        <f>D3</f>
         <v>1000</v>
       </c>
       <c r="C3" s="6">
         <v>0.8</v>
       </c>
-      <c r="D3" s="32">
-        <v>1000</v>
-      </c>
-      <c r="G3" s="32"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D3" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="E3" s="32"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="32">
-        <f>D4</f>
         <v>2700</v>
       </c>
       <c r="C4" s="6">
         <v>0.65</v>
       </c>
-      <c r="D4" s="32">
-        <v>2700</v>
-      </c>
-      <c r="G4" s="32"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D4" s="6">
+        <v>0.65</v>
+      </c>
+      <c r="E4" s="32"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" s="32">
-        <f>D5</f>
         <v>5000</v>
       </c>
       <c r="C5" s="6">
         <v>0.3</v>
       </c>
-      <c r="D5" s="32">
-        <v>5000</v>
-      </c>
-      <c r="G5" s="32"/>
+      <c r="D5" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E5" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2310,18 +2338,18 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -2332,7 +2360,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -2343,7 +2371,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -2354,7 +2382,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
@@ -2365,7 +2393,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
@@ -2376,7 +2404,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
@@ -2387,7 +2415,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
@@ -2398,7 +2426,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>2</v>

</xml_diff>